<commit_message>
Commit that goes with issue #259
</commit_message>
<xml_diff>
--- a/Blik/ProductCodes.xlsx
+++ b/Blik/ProductCodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="12195" windowHeight="6630"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="12195" windowHeight="6630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Strategische planning" sheetId="1" r:id="rId1"/>
@@ -2602,9 +2602,6 @@
     <t>ProductCode</t>
   </si>
   <si>
-    <t>CodeWerkpakket</t>
-  </si>
-  <si>
     <t>divisie</t>
   </si>
   <si>
@@ -2638,9 +2635,6 @@
     <t>doelstelling</t>
   </si>
   <si>
-    <t>[CodeWerkpakket]</t>
-  </si>
-  <si>
     <t>TO DG AGRO LN</t>
   </si>
   <si>
@@ -2651,6 +2645,12 @@
   </si>
   <si>
     <t>productcode</t>
+  </si>
+  <si>
+    <t>WerkpakketCode</t>
+  </si>
+  <si>
+    <t>[WerkpakketCode]</t>
   </si>
 </sst>
 </file>
@@ -3103,9 +3103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J380"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3119,16 +3119,16 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>479</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>475</v>
@@ -3137,24 +3137,24 @@
         <v>480</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>868</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>861</v>
+        <v>876</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>860</v>
@@ -3169,13 +3169,13 @@
         <v>292</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>478</v>
@@ -15889,7 +15889,7 @@
         <v>859</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -15973,9 +15973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15985,15 +15983,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>861</v>
+        <v>876</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>478</v>
@@ -16204,7 +16202,7 @@
         <v>211</v>
       </c>
       <c r="B28" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -16988,7 +16986,7 @@
         <v>269</v>
       </c>
       <c r="B126" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -17540,7 +17538,7 @@
         <v>131</v>
       </c>
       <c r="B195" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
This commit is meant to accompany issue #266
</commit_message>
<xml_diff>
--- a/Blik/ProductCodes.xlsx
+++ b/Blik/ProductCodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="12195" windowHeight="6630"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="12195" windowHeight="6570" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Strategische planning" sheetId="1" r:id="rId1"/>
@@ -2453,9 +2453,6 @@
     <t>voorziening</t>
   </si>
   <si>
-    <t>[Applicatie,]</t>
-  </si>
-  <si>
     <t>Incidentmanagement Crisisbeheersing</t>
   </si>
   <si>
@@ -2942,15 +2939,9 @@
     <t>Office</t>
   </si>
   <si>
-    <t>Spin,Riskbox (RACX 2015/Access),Mail,Office-excel,digital dossier,rabbit,SMG,APEX,Cros (voorheen Ebs),Fyscon,Share intern en met externen</t>
-  </si>
-  <si>
     <t>M-Spin</t>
   </si>
   <si>
-    <t>Mail,www,fax,telefoon,post,App social media,MOS,form desk,outlook (App),voice log,ISI,SPIN,Digitaal dossier,I&amp;R,PDF</t>
-  </si>
-  <si>
     <t>MOS,intranet,Excel,Spin,Spin-bedrijvenbak,Spin-L&amp;N,Maptiv,ISI,Formdesk,digitaal dossier</t>
   </si>
   <si>
@@ -2958,6 +2949,15 @@
   </si>
   <si>
     <t>Office,Spin,ISI</t>
+  </si>
+  <si>
+    <t>Spin,Riskbox (RACX 2015/Access),Mail,Office-excel,digitaal dossier,rabbit,SMG,APEX,Cros (voorheen Ebs),Fyscon,Share intern en met externen</t>
+  </si>
+  <si>
+    <t>[Voorziening,]</t>
+  </si>
+  <si>
+    <t>Mail,www,fax,telefoon,post,App social media,MOS,form desk,outlook (App),voice log,ISI,Spin,Digitaal dossier,I&amp;R,PDF</t>
   </si>
 </sst>
 </file>
@@ -3411,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J380"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
@@ -16312,7 +16312,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -16320,7 +16320,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -16328,7 +16328,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -16336,7 +16336,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -16344,7 +16344,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -16352,7 +16352,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -16360,7 +16360,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -16368,7 +16368,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -16376,7 +16376,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -16384,7 +16384,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -16392,7 +16392,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -16400,7 +16400,7 @@
         <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -16408,7 +16408,7 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -16416,7 +16416,7 @@
         <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -16424,7 +16424,7 @@
         <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -16432,7 +16432,7 @@
         <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -16440,7 +16440,7 @@
         <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -16448,7 +16448,7 @@
         <v>208</v>
       </c>
       <c r="B20" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -16456,7 +16456,7 @@
         <v>213</v>
       </c>
       <c r="B21" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -16464,7 +16464,7 @@
         <v>209</v>
       </c>
       <c r="B22" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -16472,7 +16472,7 @@
         <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -16480,7 +16480,7 @@
         <v>218</v>
       </c>
       <c r="B24" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -16488,7 +16488,7 @@
         <v>215</v>
       </c>
       <c r="B25" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -16496,7 +16496,7 @@
         <v>210</v>
       </c>
       <c r="B26" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -16504,7 +16504,7 @@
         <v>214</v>
       </c>
       <c r="B27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -16520,7 +16520,7 @@
         <v>207</v>
       </c>
       <c r="B29" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -16528,7 +16528,7 @@
         <v>216</v>
       </c>
       <c r="B30" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -16536,7 +16536,7 @@
         <v>212</v>
       </c>
       <c r="B31" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -16544,7 +16544,7 @@
         <v>204</v>
       </c>
       <c r="B32" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -16552,7 +16552,7 @@
         <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -16560,7 +16560,7 @@
         <v>206</v>
       </c>
       <c r="B34" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -16568,7 +16568,7 @@
         <v>220</v>
       </c>
       <c r="B35" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -16576,7 +16576,7 @@
         <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -16584,7 +16584,7 @@
         <v>224</v>
       </c>
       <c r="B37" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -16592,7 +16592,7 @@
         <v>228</v>
       </c>
       <c r="B38" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -16600,7 +16600,7 @@
         <v>221</v>
       </c>
       <c r="B39" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -16624,7 +16624,7 @@
         <v>194</v>
       </c>
       <c r="B42" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -16632,7 +16632,7 @@
         <v>192</v>
       </c>
       <c r="B43" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -16640,7 +16640,7 @@
         <v>225</v>
       </c>
       <c r="B44" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -16648,7 +16648,7 @@
         <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -16656,7 +16656,7 @@
         <v>223</v>
       </c>
       <c r="B46" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -16664,7 +16664,7 @@
         <v>227</v>
       </c>
       <c r="B47" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -16672,7 +16672,7 @@
         <v>271</v>
       </c>
       <c r="B48" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -16680,7 +16680,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -16688,7 +16688,7 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -16696,7 +16696,7 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -16704,7 +16704,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -16712,7 +16712,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -16720,7 +16720,7 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -16728,7 +16728,7 @@
         <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -16736,7 +16736,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -16744,7 +16744,7 @@
         <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -16752,7 +16752,7 @@
         <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -16760,7 +16760,7 @@
         <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -16768,7 +16768,7 @@
         <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -16776,7 +16776,7 @@
         <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -16784,7 +16784,7 @@
         <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -16792,7 +16792,7 @@
         <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -16800,7 +16800,7 @@
         <v>156</v>
       </c>
       <c r="B64" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -16808,7 +16808,7 @@
         <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -16816,7 +16816,7 @@
         <v>149</v>
       </c>
       <c r="B66" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -16832,7 +16832,7 @@
         <v>155</v>
       </c>
       <c r="B68" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -16840,7 +16840,7 @@
         <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -16848,7 +16848,7 @@
         <v>158</v>
       </c>
       <c r="B70" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -16856,7 +16856,7 @@
         <v>59</v>
       </c>
       <c r="B71" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -16864,7 +16864,7 @@
         <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -16872,7 +16872,7 @@
         <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -16880,7 +16880,7 @@
         <v>60</v>
       </c>
       <c r="B74" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -16888,7 +16888,7 @@
         <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -16896,7 +16896,7 @@
         <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -16904,7 +16904,7 @@
         <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -16912,7 +16912,7 @@
         <v>288</v>
       </c>
       <c r="B78" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -16920,7 +16920,7 @@
         <v>267</v>
       </c>
       <c r="B79" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -16928,7 +16928,7 @@
         <v>230</v>
       </c>
       <c r="B80" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -16936,7 +16936,7 @@
         <v>234</v>
       </c>
       <c r="B81" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -16944,7 +16944,7 @@
         <v>233</v>
       </c>
       <c r="B82" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -16952,7 +16952,7 @@
         <v>237</v>
       </c>
       <c r="B83" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -16960,7 +16960,7 @@
         <v>238</v>
       </c>
       <c r="B84" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -16968,7 +16968,7 @@
         <v>236</v>
       </c>
       <c r="B85" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -16976,7 +16976,7 @@
         <v>235</v>
       </c>
       <c r="B86" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -16984,7 +16984,7 @@
         <v>232</v>
       </c>
       <c r="B87" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -16992,7 +16992,7 @@
         <v>231</v>
       </c>
       <c r="B88" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -17000,7 +17000,7 @@
         <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -17008,7 +17008,7 @@
         <v>38</v>
       </c>
       <c r="B90" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -17016,7 +17016,7 @@
         <v>36</v>
       </c>
       <c r="B91" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -17024,7 +17024,7 @@
         <v>39</v>
       </c>
       <c r="B92" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -17032,7 +17032,7 @@
         <v>35</v>
       </c>
       <c r="B93" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -17040,7 +17040,7 @@
         <v>34</v>
       </c>
       <c r="B94" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -17048,7 +17048,7 @@
         <v>31</v>
       </c>
       <c r="B95" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -17056,7 +17056,7 @@
         <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -17064,7 +17064,7 @@
         <v>118</v>
       </c>
       <c r="B97" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -17072,7 +17072,7 @@
         <v>122</v>
       </c>
       <c r="B98" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -17080,7 +17080,7 @@
         <v>120</v>
       </c>
       <c r="B99" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -17088,7 +17088,7 @@
         <v>119</v>
       </c>
       <c r="B100" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -17096,7 +17096,7 @@
         <v>126</v>
       </c>
       <c r="B101" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -17104,7 +17104,7 @@
         <v>127</v>
       </c>
       <c r="B102" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -17112,7 +17112,7 @@
         <v>124</v>
       </c>
       <c r="B103" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -17120,7 +17120,7 @@
         <v>123</v>
       </c>
       <c r="B104" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -17128,7 +17128,7 @@
         <v>121</v>
       </c>
       <c r="B105" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -17136,7 +17136,7 @@
         <v>125</v>
       </c>
       <c r="B106" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -17144,7 +17144,7 @@
         <v>257</v>
       </c>
       <c r="B107" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -17152,7 +17152,7 @@
         <v>253</v>
       </c>
       <c r="B108" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -17160,7 +17160,7 @@
         <v>254</v>
       </c>
       <c r="B109" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -17168,7 +17168,7 @@
         <v>252</v>
       </c>
       <c r="B110" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -17176,7 +17176,7 @@
         <v>260</v>
       </c>
       <c r="B111" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -17184,7 +17184,7 @@
         <v>247</v>
       </c>
       <c r="B112" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -17192,7 +17192,7 @@
         <v>244</v>
       </c>
       <c r="B113" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -17200,7 +17200,7 @@
         <v>243</v>
       </c>
       <c r="B114" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -17208,7 +17208,7 @@
         <v>249</v>
       </c>
       <c r="B115" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
@@ -17216,7 +17216,7 @@
         <v>246</v>
       </c>
       <c r="B116" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -17224,7 +17224,7 @@
         <v>265</v>
       </c>
       <c r="B117" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -17232,7 +17232,7 @@
         <v>250</v>
       </c>
       <c r="B118" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -17240,7 +17240,7 @@
         <v>240</v>
       </c>
       <c r="B119" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
@@ -17248,7 +17248,7 @@
         <v>248</v>
       </c>
       <c r="B120" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -17256,7 +17256,7 @@
         <v>109</v>
       </c>
       <c r="B121" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -17264,7 +17264,7 @@
         <v>251</v>
       </c>
       <c r="B122" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -17272,7 +17272,7 @@
         <v>266</v>
       </c>
       <c r="B123" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -17280,7 +17280,7 @@
         <v>259</v>
       </c>
       <c r="B124" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -17288,7 +17288,7 @@
         <v>264</v>
       </c>
       <c r="B125" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -17296,7 +17296,7 @@
         <v>269</v>
       </c>
       <c r="B126" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -17304,7 +17304,7 @@
         <v>261</v>
       </c>
       <c r="B127" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
@@ -17312,7 +17312,7 @@
         <v>263</v>
       </c>
       <c r="B128" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
@@ -17320,7 +17320,7 @@
         <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -17328,7 +17328,7 @@
         <v>79</v>
       </c>
       <c r="B130" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -17336,7 +17336,7 @@
         <v>81</v>
       </c>
       <c r="B131" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -17344,7 +17344,7 @@
         <v>80</v>
       </c>
       <c r="B132" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -17352,7 +17352,7 @@
         <v>82</v>
       </c>
       <c r="B133" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -17360,7 +17360,7 @@
         <v>255</v>
       </c>
       <c r="B134" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -17368,7 +17368,7 @@
         <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -17376,7 +17376,7 @@
         <v>185</v>
       </c>
       <c r="B136" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -17384,7 +17384,7 @@
         <v>183</v>
       </c>
       <c r="B137" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -17392,7 +17392,7 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -17400,7 +17400,7 @@
         <v>186</v>
       </c>
       <c r="B139" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -17408,7 +17408,7 @@
         <v>9</v>
       </c>
       <c r="B140" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
@@ -17416,7 +17416,7 @@
         <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -17424,7 +17424,7 @@
         <v>181</v>
       </c>
       <c r="B142" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -17432,7 +17432,7 @@
         <v>187</v>
       </c>
       <c r="B143" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -17440,7 +17440,7 @@
         <v>11</v>
       </c>
       <c r="B144" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -17448,7 +17448,7 @@
         <v>258</v>
       </c>
       <c r="B145" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -17456,7 +17456,7 @@
         <v>184</v>
       </c>
       <c r="B146" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
@@ -17464,7 +17464,7 @@
         <v>188</v>
       </c>
       <c r="B147" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
@@ -17472,7 +17472,7 @@
         <v>189</v>
       </c>
       <c r="B148" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
@@ -17480,7 +17480,7 @@
         <v>182</v>
       </c>
       <c r="B149" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
@@ -17488,7 +17488,7 @@
         <v>67</v>
       </c>
       <c r="B150" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
@@ -17496,7 +17496,7 @@
         <v>72</v>
       </c>
       <c r="B151" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
@@ -17504,7 +17504,7 @@
         <v>70</v>
       </c>
       <c r="B152" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -17512,7 +17512,7 @@
         <v>71</v>
       </c>
       <c r="B153" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
@@ -17520,7 +17520,7 @@
         <v>69</v>
       </c>
       <c r="B154" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
@@ -17528,7 +17528,7 @@
         <v>73</v>
       </c>
       <c r="B155" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -17536,7 +17536,7 @@
         <v>74</v>
       </c>
       <c r="B156" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -17544,7 +17544,7 @@
         <v>75</v>
       </c>
       <c r="B157" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
@@ -17552,7 +17552,7 @@
         <v>77</v>
       </c>
       <c r="B158" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
@@ -17560,7 +17560,7 @@
         <v>68</v>
       </c>
       <c r="B159" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
@@ -17568,7 +17568,7 @@
         <v>76</v>
       </c>
       <c r="B160" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
@@ -17576,7 +17576,7 @@
         <v>86</v>
       </c>
       <c r="B161" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
@@ -17584,7 +17584,7 @@
         <v>87</v>
       </c>
       <c r="B162" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
@@ -17592,7 +17592,7 @@
         <v>90</v>
       </c>
       <c r="B163" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
@@ -17600,7 +17600,7 @@
         <v>88</v>
       </c>
       <c r="B164" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
@@ -17616,7 +17616,7 @@
         <v>85</v>
       </c>
       <c r="B166" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
@@ -17624,7 +17624,7 @@
         <v>242</v>
       </c>
       <c r="B167" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
@@ -17632,7 +17632,7 @@
         <v>241</v>
       </c>
       <c r="B168" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -17640,7 +17640,7 @@
         <v>268</v>
       </c>
       <c r="B169" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
@@ -17648,7 +17648,7 @@
         <v>256</v>
       </c>
       <c r="B170" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
@@ -17656,7 +17656,7 @@
         <v>46</v>
       </c>
       <c r="B171" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
@@ -17664,7 +17664,7 @@
         <v>45</v>
       </c>
       <c r="B172" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
@@ -17672,7 +17672,7 @@
         <v>41</v>
       </c>
       <c r="B173" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -17680,7 +17680,7 @@
         <v>42</v>
       </c>
       <c r="B174" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
@@ -17688,7 +17688,7 @@
         <v>44</v>
       </c>
       <c r="B175" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
@@ -17696,7 +17696,7 @@
         <v>170</v>
       </c>
       <c r="B176" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
@@ -17704,7 +17704,7 @@
         <v>166</v>
       </c>
       <c r="B177" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
@@ -17712,7 +17712,7 @@
         <v>163</v>
       </c>
       <c r="B178" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
@@ -17720,7 +17720,7 @@
         <v>165</v>
       </c>
       <c r="B179" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
@@ -17728,7 +17728,7 @@
         <v>168</v>
       </c>
       <c r="B180" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
@@ -17736,7 +17736,7 @@
         <v>164</v>
       </c>
       <c r="B181" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
@@ -17744,7 +17744,7 @@
         <v>162</v>
       </c>
       <c r="B182" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
@@ -17752,7 +17752,7 @@
         <v>167</v>
       </c>
       <c r="B183" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
@@ -17760,7 +17760,7 @@
         <v>169</v>
       </c>
       <c r="B184" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
@@ -17768,7 +17768,7 @@
         <v>179</v>
       </c>
       <c r="B185" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
@@ -17776,7 +17776,7 @@
         <v>172</v>
       </c>
       <c r="B186" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
@@ -17784,7 +17784,7 @@
         <v>173</v>
       </c>
       <c r="B187" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
@@ -17792,7 +17792,7 @@
         <v>176</v>
       </c>
       <c r="B188" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
@@ -17800,7 +17800,7 @@
         <v>175</v>
       </c>
       <c r="B189" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
@@ -17808,7 +17808,7 @@
         <v>177</v>
       </c>
       <c r="B190" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
@@ -17816,7 +17816,7 @@
         <v>178</v>
       </c>
       <c r="B191" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
@@ -17824,7 +17824,7 @@
         <v>174</v>
       </c>
       <c r="B192" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
@@ -17832,7 +17832,7 @@
         <v>129</v>
       </c>
       <c r="B193" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
@@ -17840,7 +17840,7 @@
         <v>130</v>
       </c>
       <c r="B194" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
@@ -17848,7 +17848,7 @@
         <v>131</v>
       </c>
       <c r="B195" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
@@ -17856,7 +17856,7 @@
         <v>285</v>
       </c>
       <c r="B196" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
@@ -17864,7 +17864,7 @@
         <v>290</v>
       </c>
       <c r="B197" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
@@ -17872,7 +17872,7 @@
         <v>279</v>
       </c>
       <c r="B198" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
@@ -17880,7 +17880,7 @@
         <v>278</v>
       </c>
       <c r="B199" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
@@ -17888,7 +17888,7 @@
         <v>275</v>
       </c>
       <c r="B200" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
@@ -17896,7 +17896,7 @@
         <v>202</v>
       </c>
       <c r="B201" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
@@ -17904,7 +17904,7 @@
         <v>274</v>
       </c>
       <c r="B202" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
@@ -17912,7 +17912,7 @@
         <v>289</v>
       </c>
       <c r="B203" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
@@ -17920,7 +17920,7 @@
         <v>280</v>
       </c>
       <c r="B204" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
@@ -17928,7 +17928,7 @@
         <v>282</v>
       </c>
       <c r="B205" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
@@ -17936,7 +17936,7 @@
         <v>277</v>
       </c>
       <c r="B206" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
@@ -17944,7 +17944,7 @@
         <v>272</v>
       </c>
       <c r="B207" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
@@ -17952,7 +17952,7 @@
         <v>281</v>
       </c>
       <c r="B208" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
@@ -17960,7 +17960,7 @@
         <v>273</v>
       </c>
       <c r="B209" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
@@ -17968,7 +17968,7 @@
         <v>287</v>
       </c>
       <c r="B210" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
@@ -17976,7 +17976,7 @@
         <v>276</v>
       </c>
       <c r="B211" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
@@ -17984,7 +17984,7 @@
         <v>286</v>
       </c>
       <c r="B212" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
@@ -17992,7 +17992,7 @@
         <v>291</v>
       </c>
       <c r="B213" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
@@ -18000,7 +18000,7 @@
         <v>283</v>
       </c>
       <c r="B214" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
@@ -18008,7 +18008,7 @@
         <v>100</v>
       </c>
       <c r="B215" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
@@ -18016,7 +18016,7 @@
         <v>94</v>
       </c>
       <c r="B216" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
@@ -18024,7 +18024,7 @@
         <v>108</v>
       </c>
       <c r="B217" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
@@ -18032,7 +18032,7 @@
         <v>96</v>
       </c>
       <c r="B218" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
@@ -18040,7 +18040,7 @@
         <v>107</v>
       </c>
       <c r="B219" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
@@ -18048,7 +18048,7 @@
         <v>95</v>
       </c>
       <c r="B220" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
@@ -18056,7 +18056,7 @@
         <v>99</v>
       </c>
       <c r="B221" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
@@ -18064,7 +18064,7 @@
         <v>97</v>
       </c>
       <c r="B222" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
@@ -18072,7 +18072,7 @@
         <v>98</v>
       </c>
       <c r="B223" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
@@ -18080,7 +18080,7 @@
         <v>93</v>
       </c>
       <c r="B224" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
@@ -18088,7 +18088,7 @@
         <v>104</v>
       </c>
       <c r="B225" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
@@ -18096,7 +18096,7 @@
         <v>102</v>
       </c>
       <c r="B226" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
@@ -18104,7 +18104,7 @@
         <v>103</v>
       </c>
       <c r="B227" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
@@ -18112,7 +18112,7 @@
         <v>106</v>
       </c>
       <c r="B228" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
@@ -18120,7 +18120,7 @@
         <v>105</v>
       </c>
       <c r="B229" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
@@ -18136,7 +18136,7 @@
         <v>198</v>
       </c>
       <c r="B231" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
@@ -18144,7 +18144,7 @@
         <v>200</v>
       </c>
       <c r="B232" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
@@ -18152,7 +18152,7 @@
         <v>262</v>
       </c>
       <c r="B233" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
@@ -18160,7 +18160,7 @@
         <v>133</v>
       </c>
       <c r="B234" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
@@ -18168,7 +18168,7 @@
         <v>137</v>
       </c>
       <c r="B235" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
@@ -18176,7 +18176,7 @@
         <v>144</v>
       </c>
       <c r="B236" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
@@ -18184,7 +18184,7 @@
         <v>136</v>
       </c>
       <c r="B237" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
@@ -18192,7 +18192,7 @@
         <v>134</v>
       </c>
       <c r="B238" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
@@ -18200,7 +18200,7 @@
         <v>146</v>
       </c>
       <c r="B239" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
@@ -18208,7 +18208,7 @@
         <v>142</v>
       </c>
       <c r="B240" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
@@ -18216,7 +18216,7 @@
         <v>143</v>
       </c>
       <c r="B241" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
@@ -18224,7 +18224,7 @@
         <v>135</v>
       </c>
       <c r="B242" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
@@ -18232,7 +18232,7 @@
         <v>139</v>
       </c>
       <c r="B243" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
@@ -18240,7 +18240,7 @@
         <v>145</v>
       </c>
       <c r="B244" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
@@ -18248,7 +18248,7 @@
         <v>284</v>
       </c>
       <c r="B245" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
@@ -18256,7 +18256,7 @@
         <v>141</v>
       </c>
       <c r="B246" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
@@ -18264,7 +18264,7 @@
         <v>147</v>
       </c>
       <c r="B247" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
   </sheetData>
@@ -18279,8 +18279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18325,7 +18325,7 @@
         <v>806</v>
       </c>
       <c r="F2" t="s">
-        <v>811</v>
+        <v>978</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -18342,7 +18342,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -18428,7 +18428,7 @@
         <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -18448,7 +18448,7 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -18468,7 +18468,7 @@
         <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -18488,7 +18488,7 @@
         <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -18508,7 +18508,7 @@
         <v>608</v>
       </c>
       <c r="F14" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -18576,7 +18576,7 @@
         <v>116</v>
       </c>
       <c r="F19" t="s">
-        <v>974</v>
+        <v>977</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -18596,7 +18596,7 @@
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -18696,7 +18696,7 @@
         <v>543</v>
       </c>
       <c r="F27" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -18746,7 +18746,7 @@
         <v>751</v>
       </c>
       <c r="F31" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -18843,7 +18843,7 @@
         <v>151</v>
       </c>
       <c r="F39" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -18851,7 +18851,7 @@
         <v>738</v>
       </c>
       <c r="B40" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C40" t="s">
         <v>751</v>
@@ -18863,7 +18863,7 @@
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -18888,7 +18888,7 @@
         <v>739</v>
       </c>
       <c r="B42" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C42" t="s">
         <v>751</v>
@@ -18900,7 +18900,7 @@
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
make Arch.adl compilable again.
</commit_message>
<xml_diff>
--- a/Blik/ProductCodes.xlsx
+++ b/Blik/ProductCodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="12195" windowHeight="6510" tabRatio="731" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="210" windowWidth="12195" windowHeight="6510" tabRatio="731" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Strategische planning" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="1912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4751" uniqueCount="1908">
   <si>
     <t>Divisie</t>
   </si>
@@ -5169,9 +5169,6 @@
     <t>zt18</t>
   </si>
   <si>
-    <t>Art. 1:3 lid 3 AwB</t>
-  </si>
-  <si>
     <t>definitie</t>
   </si>
   <si>
@@ -5229,9 +5226,6 @@
     <t>voorschrift</t>
   </si>
   <si>
-    <t>Wetsartikel</t>
-  </si>
-  <si>
     <t>plaats</t>
   </si>
   <si>
@@ -5292,21 +5286,6 @@
     <t>uitgereikt</t>
   </si>
   <si>
-    <t>Art. 5:48 lid 3 Awb</t>
-  </si>
-  <si>
-    <t>Art. 5:9 Awb</t>
-  </si>
-  <si>
-    <t>Art. 5:9 sub b. Awb</t>
-  </si>
-  <si>
-    <t>Art. 5:9 sub a. Awb</t>
-  </si>
-  <si>
-    <t>Art. 9:1 AwB</t>
-  </si>
-  <si>
     <t>[Klacht]</t>
   </si>
   <si>
@@ -5481,51 +5460,9 @@
     <t>inspecteur medewerker toezicht van de Afdeling Toezichtuitvoering Plant en Natuur</t>
   </si>
   <si>
-    <t>Art 1 sub a. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub b. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub c. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub d. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub e. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub f. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub g. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub h. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub i. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub j. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub k. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub l. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
-    <t>Art 1 sub m. Besluit mandaat, volmacht en machtiging van de inspecteur-generaal van de Nederlandse Voedsel- en Warenautoriteit van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>Vergunning</t>
   </si>
   <si>
-    <t>Art. 5 WaW</t>
-  </si>
-  <si>
     <t>Een vergunning is een beschikking waarin aan een persoon een afwijking op regelgeving wordt toegestaan of een bij regelgeving vereiste toestemming wordt verleend.</t>
   </si>
   <si>
@@ -5592,114 +5529,48 @@
     <t>Directie Staf</t>
   </si>
   <si>
-    <t>Art XVII lid 3 Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 3 sub b. Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 3 sub d. Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 3 sub e. Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 3 sub f. Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 3 sub g. Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 3 sub a. Besluit mandaat, volmacht en machtiging EZ 2015</t>
-  </si>
-  <si>
-    <t>Art XVII lid 2 sub a. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>werken aan de veiligheid van voedsel- en niet-voedsel producten om de gezondheid van mens en dier te beschermen</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub b. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>zorg dragen voor handhaving van wet- en regelgeving waarvoor de minister (mede) verantwoordelijkheid draagt op het terrein van land- en tuinbouw, natuur, visserij, diergezondheid en welzijn, milieu, dierproeven, voedselveiligheid en consumentenproducten</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub c. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>verzamelen en verdelen van inlichtingen en het uitvoeren van analyses ter vergroting van inzicht, aard en omvang van (niet-)naleving</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub d. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>informeren van de buitenwereld over risico's en risicoreductie</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub e. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>fungeren als centraal meldpunt voor consumenten, bedrijven, laboratoria, de Europese Commissie en andere landen op het gebied van voedselveiligheid</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub f. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>samenwerken met de Europese Voedsel Veiligheidsautoriteit</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub g. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>bewaken en bevorderen van de gezondheid van planten waarmee een bijdrage wordt geleverd aan een gezonde groene sector van internationaal aanzien, een gezonde en veilige land- en tuinbouw en een landschap met een hoge biodiversiteit</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub h. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>voorkomen dat ziekten, plagen en ongewenste planten binnen Nederland en over de wereld worden verspreid</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub i. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>bevorderen dat planten, ziekten, plagen en onkruiden op een veilige en duurzame wijze worden beheerst</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub j. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>optreden als coördinerend controle orgaan voor het Gemeenschappelijk Landbouwbeleid</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub k. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>uitoefenen van verificaties en controles van het Gemeenschappelijk Landbouwbeleid</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub l. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>verlenen van ontheffingen van maatregelen ter bestrijding van plantenziekten op grond van de Invoeringswet openbare lichamen Bonaire, Sint Eustatius en Saba</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub m. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>verrichten van taken waaronder het verlenen, schorsen en intrekken van ontheffingen, erkenningen, vergunningen, het nemen van maatregelen en het doen van aanwijzingen op het terrein van de Gezondheids- en welzijnswet voor dieren, de Wet gewasbeschermingsmiddelen en biociden, de Wet dieren, de Plantenziektenwet, de Landbouwwet, de Landbouwkwaliteitswet, de Flora- en Faunawet, visserijregelgeving en de daarmee samenhangende besluiten</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub n. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>ontwikkelen van de kennisagenda en ondersteunen divisies bij strategische kennisontwikkeling</t>
   </si>
   <si>
-    <t>Art XVII lid 2 sub o. Besluit mandaat, volmacht en machtiging van het Ministerie van Economische Zaken 2015</t>
-  </si>
-  <si>
     <t>verzorgen van opleidingen voor managers en (bij)scholing voor handhavers op het gebied van toezicht en opsporing.</t>
   </si>
   <si>
@@ -5773,6 +5644,123 @@
   </si>
   <si>
     <t>projectmedewerker</t>
+  </si>
+  <si>
+    <t>486</t>
+  </si>
+  <si>
+    <t>487</t>
+  </si>
+  <si>
+    <t>488</t>
+  </si>
+  <si>
+    <t>489</t>
+  </si>
+  <si>
+    <t>490</t>
+  </si>
+  <si>
+    <t>491</t>
+  </si>
+  <si>
+    <t>492</t>
+  </si>
+  <si>
+    <t>493</t>
+  </si>
+  <si>
+    <t>494</t>
+  </si>
+  <si>
+    <t>495</t>
+  </si>
+  <si>
+    <t>496</t>
+  </si>
+  <si>
+    <t>497</t>
+  </si>
+  <si>
+    <t>498</t>
+  </si>
+  <si>
+    <t>499</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>501</t>
+  </si>
+  <si>
+    <t>502</t>
+  </si>
+  <si>
+    <t>503</t>
+  </si>
+  <si>
+    <t>504</t>
+  </si>
+  <si>
+    <t>505</t>
+  </si>
+  <si>
+    <t>506</t>
+  </si>
+  <si>
+    <t>507</t>
+  </si>
+  <si>
+    <t>508</t>
+  </si>
+  <si>
+    <t>509</t>
+  </si>
+  <si>
+    <t>510</t>
+  </si>
+  <si>
+    <t>511</t>
+  </si>
+  <si>
+    <t>512</t>
+  </si>
+  <si>
+    <t>513</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>515</t>
+  </si>
+  <si>
+    <t>516</t>
+  </si>
+  <si>
+    <t>517</t>
+  </si>
+  <si>
+    <t>518</t>
+  </si>
+  <si>
+    <t>519</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>521</t>
+  </si>
+  <si>
+    <t>522</t>
+  </si>
+  <si>
+    <t>523</t>
+  </si>
+  <si>
+    <t>524</t>
   </si>
 </sst>
 </file>
@@ -5790,6 +5778,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -18849,123 +18838,123 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C3" t="s">
         <v>1714</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1715</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1716</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C4" t="s">
         <v>1717</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1718</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1719</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C5" t="s">
         <v>1720</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1721</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1722</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C6" t="s">
         <v>1723</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1724</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1725</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C7" t="s">
         <v>1726</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>1727</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1728</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D8" t="s">
         <v>1735</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1736</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1737</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D9" t="s">
         <v>1741</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1742</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1743</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1743</v>
+      </c>
+      <c r="D10" t="s">
         <v>1744</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1745</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1746</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D11" t="s">
         <v>1747</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1748</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1749</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>1771</v>
+        <v>1764</v>
       </c>
       <c r="C12" t="s">
-        <v>1772</v>
+        <v>1765</v>
       </c>
       <c r="D12" t="s">
-        <v>1773</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>1780</v>
+        <v>1773</v>
       </c>
       <c r="C13" t="s">
-        <v>1781</v>
+        <v>1774</v>
       </c>
       <c r="D13" t="s">
-        <v>1782</v>
+        <v>1775</v>
       </c>
     </row>
   </sheetData>
@@ -18985,34 +18974,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1756</v>
+        <v>1749</v>
       </c>
       <c r="B1" t="s">
-        <v>1757</v>
+        <v>1750</v>
       </c>
       <c r="C1" t="s">
-        <v>1759</v>
+        <v>1752</v>
       </c>
       <c r="D1" t="s">
         <v>1589</v>
       </c>
       <c r="E1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1759</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="J1" t="s">
         <v>1762</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1766</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1765</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1767</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1768</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1769</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -19020,7 +19009,7 @@
         <v>1678</v>
       </c>
       <c r="B2" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="C2" t="s">
         <v>706</v>
@@ -19029,36 +19018,36 @@
         <v>319</v>
       </c>
       <c r="E2" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1756</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="J2" t="s">
         <v>1763</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1763</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1770</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>1758</v>
+        <v>1751</v>
       </c>
       <c r="C3" t="s">
-        <v>1761</v>
+        <v>1754</v>
       </c>
       <c r="D3" t="s">
-        <v>1760</v>
+        <v>1753</v>
       </c>
       <c r="E3" t="s">
-        <v>1764</v>
+        <v>1757</v>
       </c>
     </row>
   </sheetData>
@@ -19076,24 +19065,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1777</v>
+        <v>1770</v>
       </c>
       <c r="B1" t="s">
-        <v>1778</v>
+        <v>1771</v>
       </c>
       <c r="C1" t="s">
-        <v>1779</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1777</v>
+        <v>1770</v>
       </c>
       <c r="B2" t="s">
-        <v>1771</v>
+        <v>1764</v>
       </c>
       <c r="C2" t="s">
-        <v>1763</v>
+        <v>1756</v>
       </c>
     </row>
   </sheetData>
@@ -19111,27 +19100,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1780</v>
+        <v>1773</v>
       </c>
       <c r="B1" t="s">
-        <v>1774</v>
+        <v>1767</v>
       </c>
       <c r="C1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D1" t="s">
         <v>1776</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1783</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1780</v>
+        <v>1773</v>
       </c>
       <c r="B2" t="s">
-        <v>1775</v>
+        <v>1768</v>
       </c>
       <c r="C2" t="s">
-        <v>1763</v>
+        <v>1756</v>
       </c>
     </row>
   </sheetData>
@@ -19149,16 +19138,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="20" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1792</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1791</v>
+        <v>1785</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1784</v>
       </c>
       <c r="C1" t="s">
         <v>807</v>
@@ -19168,8 +19157,8 @@
       <c r="A2" t="s">
         <v>985</v>
       </c>
-      <c r="B2" t="s">
-        <v>1905</v>
+      <c r="B2" s="20" t="s">
+        <v>1862</v>
       </c>
       <c r="C2" t="s">
         <v>319</v>
@@ -19177,151 +19166,151 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1793</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1814</v>
+        <v>1786</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1869</v>
       </c>
       <c r="C3" t="s">
-        <v>1784</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1794</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1815</v>
+        <v>1787</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>1870</v>
       </c>
       <c r="C4" t="s">
-        <v>1785</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1795</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1816</v>
+        <v>1788</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>1871</v>
       </c>
       <c r="C5" t="s">
-        <v>1806</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1796</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1817</v>
+        <v>1789</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>1872</v>
       </c>
       <c r="C6" t="s">
-        <v>1807</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1797</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1818</v>
+        <v>1790</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>1873</v>
       </c>
       <c r="C7" t="s">
-        <v>1808</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1798</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1819</v>
+        <v>1791</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>1874</v>
       </c>
       <c r="C8" t="s">
-        <v>1786</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1799</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1820</v>
+        <v>1792</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>1875</v>
       </c>
       <c r="C9" t="s">
-        <v>1787</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1800</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1821</v>
+        <v>1793</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>1876</v>
       </c>
       <c r="C10" t="s">
-        <v>1809</v>
+        <v>1802</v>
       </c>
       <c r="D10" t="s">
-        <v>1788</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1801</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1822</v>
+        <v>1794</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>1877</v>
       </c>
       <c r="C11" t="s">
-        <v>1789</v>
+        <v>1782</v>
       </c>
       <c r="D11" t="s">
-        <v>1790</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1802</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1823</v>
+        <v>1795</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>1878</v>
       </c>
       <c r="C12" t="s">
-        <v>1810</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1803</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1824</v>
+        <v>1796</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>1879</v>
       </c>
       <c r="C13" t="s">
-        <v>1811</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1825</v>
+        <v>1797</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>1880</v>
       </c>
       <c r="C14" t="s">
-        <v>1812</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1805</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1826</v>
+        <v>1798</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>1881</v>
       </c>
       <c r="C15" t="s">
-        <v>1813</v>
+        <v>1806</v>
       </c>
     </row>
   </sheetData>
@@ -19333,9 +19322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19344,21 +19331,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1908</v>
+        <v>1865</v>
       </c>
       <c r="B1" t="s">
         <v>807</v>
       </c>
       <c r="C1" t="s">
-        <v>1849</v>
+        <v>1828</v>
       </c>
       <c r="D1" t="s">
-        <v>1791</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1907</v>
+        <v>1864</v>
       </c>
       <c r="B2" t="s">
         <v>319</v>
@@ -19367,119 +19354,119 @@
         <v>319</v>
       </c>
       <c r="D2" t="s">
-        <v>1905</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1830</v>
+        <v>1809</v>
       </c>
       <c r="B3" t="s">
-        <v>1838</v>
+        <v>1817</v>
       </c>
       <c r="C3" t="s">
         <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>1851</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1831</v>
+        <v>1810</v>
       </c>
       <c r="B4" t="s">
-        <v>1839</v>
+        <v>1818</v>
       </c>
       <c r="C4" t="s">
-        <v>1848</v>
+        <v>1827</v>
       </c>
       <c r="D4" t="s">
-        <v>1852</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1832</v>
+        <v>1811</v>
       </c>
       <c r="B5" t="s">
-        <v>1840</v>
+        <v>1819</v>
       </c>
       <c r="C5" t="s">
         <v>816</v>
       </c>
       <c r="D5" t="s">
-        <v>1853</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1833</v>
+        <v>1812</v>
       </c>
       <c r="B6" t="s">
-        <v>1841</v>
+        <v>1820</v>
       </c>
       <c r="C6" t="s">
-        <v>1842</v>
+        <v>1821</v>
       </c>
       <c r="D6" t="s">
-        <v>1853</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1834</v>
+        <v>1813</v>
       </c>
       <c r="B7" t="s">
-        <v>1843</v>
+        <v>1822</v>
       </c>
       <c r="C7" t="s">
-        <v>1844</v>
+        <v>1823</v>
       </c>
       <c r="D7" t="s">
-        <v>1854</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1835</v>
+        <v>1814</v>
       </c>
       <c r="B8" t="s">
-        <v>1845</v>
+        <v>1824</v>
       </c>
       <c r="C8" t="s">
-        <v>1846</v>
+        <v>1825</v>
       </c>
       <c r="D8" t="s">
-        <v>1855</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1836</v>
+        <v>1815</v>
       </c>
       <c r="B9" t="s">
-        <v>1847</v>
+        <v>1826</v>
       </c>
       <c r="C9" t="s">
         <v>298</v>
       </c>
       <c r="D9" t="s">
-        <v>1856</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1837</v>
+        <v>1816</v>
       </c>
       <c r="B10" t="s">
-        <v>1850</v>
+        <v>1829</v>
       </c>
       <c r="C10" t="s">
-        <v>1909</v>
+        <v>1866</v>
       </c>
       <c r="D10" t="s">
-        <v>1857</v>
+        <v>1907</v>
       </c>
     </row>
   </sheetData>
@@ -22519,9 +22506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22592,7 +22577,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>1400</v>
       </c>
@@ -22627,7 +22612,7 @@
         <v>987</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>1238</v>
@@ -22646,7 +22631,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>1402</v>
       </c>
@@ -22654,7 +22639,7 @@
         <v>987</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>1239</v>
@@ -22673,7 +22658,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>1403</v>
       </c>
@@ -22700,7 +22685,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>1404</v>
       </c>
@@ -22727,7 +22712,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>1405</v>
       </c>
@@ -22752,7 +22737,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>1406</v>
       </c>
@@ -22779,7 +22764,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>1407</v>
       </c>
@@ -22806,7 +22791,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>1408</v>
       </c>
@@ -22833,7 +22818,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>1409</v>
       </c>
@@ -22860,7 +22845,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>1410</v>
       </c>
@@ -22887,7 +22872,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>1411</v>
       </c>
@@ -22916,7 +22901,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>1412</v>
       </c>
@@ -22945,7 +22930,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>1413</v>
       </c>
@@ -22972,7 +22957,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>1414</v>
       </c>
@@ -22999,7 +22984,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>1415</v>
       </c>
@@ -23026,7 +23011,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>1416</v>
       </c>
@@ -23055,7 +23040,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>1417</v>
       </c>
@@ -23082,7 +23067,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>1418</v>
       </c>
@@ -23109,7 +23094,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>1419</v>
       </c>
@@ -23117,7 +23102,7 @@
         <v>987</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>1241</v>
@@ -23136,7 +23121,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>1420</v>
       </c>
@@ -23144,7 +23129,7 @@
         <v>987</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>1241</v>
@@ -23163,7 +23148,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>1421</v>
       </c>
@@ -23190,7 +23175,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>1422</v>
       </c>
@@ -23217,7 +23202,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>1423</v>
       </c>
@@ -23244,7 +23229,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>1424</v>
       </c>
@@ -23271,7 +23256,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>1425</v>
       </c>
@@ -23298,7 +23283,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>1426</v>
       </c>
@@ -23325,7 +23310,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>1427</v>
       </c>
@@ -23354,7 +23339,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>1428</v>
       </c>
@@ -23381,7 +23366,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>1429</v>
       </c>
@@ -23408,7 +23393,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>1430</v>
       </c>
@@ -23435,7 +23420,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>1431</v>
       </c>
@@ -23460,7 +23445,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>1432</v>
       </c>
@@ -23485,7 +23470,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>1433</v>
       </c>
@@ -23510,7 +23495,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>1434</v>
       </c>
@@ -23535,7 +23520,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>1435</v>
       </c>
@@ -23560,7 +23545,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>1436</v>
       </c>
@@ -23585,7 +23570,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>1437</v>
       </c>
@@ -23612,7 +23597,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>1438</v>
       </c>
@@ -23639,7 +23624,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>1439</v>
       </c>
@@ -23664,7 +23649,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>1440</v>
       </c>
@@ -23689,7 +23674,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>1441</v>
       </c>
@@ -23714,7 +23699,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>1442</v>
       </c>
@@ -23739,7 +23724,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>1443</v>
       </c>
@@ -23766,7 +23751,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>1444</v>
       </c>
@@ -23793,7 +23778,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>1445</v>
       </c>
@@ -23818,7 +23803,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>1446</v>
       </c>
@@ -23826,7 +23811,7 @@
         <v>1022</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>1245</v>
@@ -23845,7 +23830,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>1447</v>
       </c>
@@ -23870,7 +23855,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>1448</v>
       </c>
@@ -23897,7 +23882,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>1449</v>
       </c>
@@ -23924,7 +23909,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>1450</v>
       </c>
@@ -23932,7 +23917,7 @@
         <v>1022</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>1248</v>
@@ -23951,7 +23936,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>1451</v>
       </c>
@@ -23980,7 +23965,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>1452</v>
       </c>
@@ -24007,7 +23992,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>1453</v>
       </c>
@@ -24034,7 +24019,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>1454</v>
       </c>
@@ -24063,7 +24048,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>1455</v>
       </c>
@@ -24090,7 +24075,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>1456</v>
       </c>
@@ -24098,7 +24083,7 @@
         <v>1022</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>1250</v>
@@ -24115,7 +24100,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>1457</v>
       </c>
@@ -24123,7 +24108,7 @@
         <v>1044</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>1910</v>
+        <v>1867</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>1223</v>
@@ -24142,7 +24127,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>1458</v>
       </c>
@@ -24150,7 +24135,7 @@
         <v>1044</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>1910</v>
+        <v>1867</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>1226</v>
@@ -24169,7 +24154,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>1459</v>
       </c>
@@ -24177,7 +24162,7 @@
         <v>1044</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>1252</v>
@@ -24198,7 +24183,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>1460</v>
       </c>
@@ -24223,7 +24208,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>1461</v>
       </c>
@@ -24250,7 +24235,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>1462</v>
       </c>
@@ -24258,7 +24243,7 @@
         <v>1044</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>1910</v>
+        <v>1867</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>1229</v>
@@ -24275,7 +24260,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>1463</v>
       </c>
@@ -24300,7 +24285,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>1464</v>
       </c>
@@ -24308,7 +24293,7 @@
         <v>1044</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>1910</v>
+        <v>1867</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>1231</v>
@@ -24327,7 +24312,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>1465</v>
       </c>
@@ -24335,7 +24320,7 @@
         <v>1044</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>1256</v>
@@ -24354,7 +24339,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>1466</v>
       </c>
@@ -24381,7 +24366,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>1467</v>
       </c>
@@ -24408,7 +24393,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
         <v>1468</v>
       </c>
@@ -24435,7 +24420,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>1469</v>
       </c>
@@ -24464,7 +24449,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>1470</v>
       </c>
@@ -24472,7 +24457,7 @@
         <v>1044</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>1258</v>
@@ -24491,7 +24476,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>1471</v>
       </c>
@@ -24499,7 +24484,7 @@
         <v>1044</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>1910</v>
+        <v>1867</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>1234</v>
@@ -24518,7 +24503,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
         <v>1472</v>
       </c>
@@ -24526,7 +24511,7 @@
         <v>1044</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>1260</v>
@@ -24547,7 +24532,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>1473</v>
       </c>
@@ -24555,7 +24540,7 @@
         <v>1044</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>1263</v>
@@ -24576,7 +24561,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>1474</v>
       </c>
@@ -24584,7 +24569,7 @@
         <v>1044</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>1910</v>
+        <v>1867</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>1236</v>
@@ -24603,7 +24588,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>1475</v>
       </c>
@@ -24611,7 +24596,7 @@
         <v>1044</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>1266</v>
@@ -24630,7 +24615,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
         <v>1476</v>
       </c>
@@ -24638,7 +24623,7 @@
         <v>1044</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>1268</v>
@@ -24657,7 +24642,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>1477</v>
       </c>
@@ -24665,7 +24650,7 @@
         <v>1044</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>1270</v>
@@ -24686,7 +24671,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>1478</v>
       </c>
@@ -24694,7 +24679,7 @@
         <v>1044</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>1273</v>
@@ -24713,7 +24698,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>1479</v>
       </c>
@@ -24740,7 +24725,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
         <v>1480</v>
       </c>
@@ -24748,7 +24733,7 @@
         <v>1044</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>1276</v>
@@ -24773,7 +24758,7 @@
         <v>1044</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>1911</v>
+        <v>1868</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>1280</v>
@@ -24792,7 +24777,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>1482</v>
       </c>
@@ -24800,7 +24785,7 @@
         <v>1044</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>1906</v>
+        <v>1863</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>1277</v>
@@ -24846,7 +24831,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
         <v>1484</v>
       </c>
@@ -24871,7 +24856,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
         <v>1485</v>
       </c>
@@ -24896,7 +24881,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
         <v>1486</v>
       </c>
@@ -24919,7 +24904,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
         <v>1487</v>
       </c>
@@ -24944,7 +24929,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
         <v>1488</v>
       </c>
@@ -24967,7 +24952,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A92" s="9" t="s">
         <v>1489</v>
       </c>
@@ -24994,7 +24979,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
         <v>1490</v>
       </c>
@@ -25019,7 +25004,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
         <v>1491</v>
       </c>
@@ -25044,7 +25029,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>1492</v>
       </c>
@@ -25071,7 +25056,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A96" s="9" t="s">
         <v>1493</v>
       </c>
@@ -25094,7 +25079,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="9" t="s">
         <v>1494</v>
       </c>
@@ -25119,7 +25104,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
         <v>1495</v>
       </c>
@@ -25146,7 +25131,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
         <v>1496</v>
       </c>
@@ -25171,7 +25156,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
         <v>1497</v>
       </c>
@@ -25196,7 +25181,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
         <v>1498</v>
       </c>
@@ -25219,7 +25204,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>1499</v>
       </c>
@@ -25244,7 +25229,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>1500</v>
       </c>
@@ -25269,7 +25254,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
         <v>1501</v>
       </c>
@@ -25296,7 +25281,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
         <v>1502</v>
       </c>
@@ -25321,7 +25306,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
         <v>1503</v>
       </c>
@@ -25346,7 +25331,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
         <v>1504</v>
       </c>
@@ -25371,7 +25356,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
         <v>1505</v>
       </c>
@@ -25398,7 +25383,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
         <v>1506</v>
       </c>
@@ -25423,7 +25408,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A110" s="9" t="s">
         <v>1507</v>
       </c>
@@ -25448,7 +25433,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
         <v>1508</v>
       </c>
@@ -25473,7 +25458,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
         <v>1509</v>
       </c>
@@ -25498,7 +25483,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
         <v>1510</v>
       </c>
@@ -25523,7 +25508,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="9" t="s">
         <v>1511</v>
       </c>
@@ -25544,7 +25529,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
         <v>1512</v>
       </c>
@@ -25569,7 +25554,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
         <v>1513</v>
       </c>
@@ -25594,7 +25579,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
         <v>1514</v>
       </c>
@@ -25621,7 +25606,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A118" s="9" t="s">
         <v>1515</v>
       </c>
@@ -25648,7 +25633,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
         <v>1516</v>
       </c>
@@ -25673,7 +25658,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
         <v>1517</v>
       </c>
@@ -25698,7 +25683,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
         <v>1518</v>
       </c>
@@ -25723,7 +25708,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="9" t="s">
         <v>1519</v>
       </c>
@@ -25748,7 +25733,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
         <v>1520</v>
       </c>
@@ -25775,7 +25760,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
         <v>1521</v>
       </c>
@@ -25800,7 +25785,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
         <v>1522</v>
       </c>
@@ -25825,7 +25810,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
         <v>1523</v>
       </c>
@@ -25850,7 +25835,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
         <v>1524</v>
       </c>
@@ -25875,7 +25860,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
         <v>1525</v>
       </c>
@@ -25902,7 +25887,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
         <v>1526</v>
       </c>
@@ -25929,7 +25914,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A130" s="9" t="s">
         <v>1527</v>
       </c>
@@ -25954,7 +25939,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A131" s="9" t="s">
         <v>1528</v>
       </c>
@@ -25979,7 +25964,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A132" s="9" t="s">
         <v>1529</v>
       </c>
@@ -26004,7 +25989,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A133" s="9" t="s">
         <v>1530</v>
       </c>
@@ -26029,7 +26014,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A134" s="9" t="s">
         <v>1531</v>
       </c>
@@ -26054,7 +26039,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
         <v>1532</v>
       </c>
@@ -26081,7 +26066,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A136" s="9" t="s">
         <v>1533</v>
       </c>
@@ -26106,7 +26091,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A137" s="9" t="s">
         <v>1534</v>
       </c>
@@ -26131,7 +26116,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A138" s="9" t="s">
         <v>1535</v>
       </c>
@@ -26156,7 +26141,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
         <v>1536</v>
       </c>
@@ -26181,7 +26166,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A140" s="9" t="s">
         <v>1537</v>
       </c>
@@ -26206,7 +26191,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A141" s="9" t="s">
         <v>1538</v>
       </c>
@@ -26231,7 +26216,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A142" s="9" t="s">
         <v>1539</v>
       </c>
@@ -26256,7 +26241,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A143" s="9" t="s">
         <v>1540</v>
       </c>
@@ -26281,7 +26266,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>1541</v>
       </c>
@@ -26306,7 +26291,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A145" s="9" t="s">
         <v>1542</v>
       </c>
@@ -26333,7 +26318,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A146" s="9" t="s">
         <v>1543</v>
       </c>
@@ -26358,7 +26343,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A147" s="9" t="s">
         <v>1544</v>
       </c>
@@ -26383,7 +26368,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A148" s="9" t="s">
         <v>1545</v>
       </c>
@@ -26408,7 +26393,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>1546</v>
       </c>
@@ -26433,7 +26418,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A150" s="9" t="s">
         <v>1547</v>
       </c>
@@ -26456,7 +26441,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
         <v>1548</v>
       </c>
@@ -26481,7 +26466,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A152" s="9" t="s">
         <v>1549</v>
       </c>
@@ -26504,7 +26489,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A153" s="9" t="s">
         <v>1550</v>
       </c>
@@ -26529,7 +26514,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A154" s="9" t="s">
         <v>1551</v>
       </c>
@@ -26552,7 +26537,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A155" s="9" t="s">
         <v>1552</v>
       </c>
@@ -26577,7 +26562,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A156" s="9" t="s">
         <v>1553</v>
       </c>
@@ -26604,7 +26589,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A157" s="9" t="s">
         <v>1554</v>
       </c>
@@ -26631,7 +26616,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A158" s="9" t="s">
         <v>1555</v>
       </c>
@@ -26658,7 +26643,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A159" s="9" t="s">
         <v>1556</v>
       </c>
@@ -26685,7 +26670,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A160" s="9" t="s">
         <v>1557</v>
       </c>
@@ -26712,7 +26697,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A161" s="9" t="s">
         <v>1558</v>
       </c>
@@ -26739,7 +26724,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A162" s="9" t="s">
         <v>1559</v>
       </c>
@@ -26766,7 +26751,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A163" s="9" t="s">
         <v>1560</v>
       </c>
@@ -26793,7 +26778,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A164" s="9" t="s">
         <v>1561</v>
       </c>
@@ -26820,7 +26805,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A165" s="9" t="s">
         <v>1562</v>
       </c>
@@ -26874,7 +26859,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A167" s="9" t="s">
         <v>1564</v>
       </c>
@@ -26901,7 +26886,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
         <v>1565</v>
       </c>
@@ -26982,7 +26967,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A171" s="9" t="s">
         <v>1568</v>
       </c>
@@ -27009,7 +26994,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A172" s="9" t="s">
         <v>1569</v>
       </c>
@@ -27090,7 +27075,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A175" s="9" t="s">
         <v>1572</v>
       </c>
@@ -27117,7 +27102,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A176" s="9" t="s">
         <v>1573</v>
       </c>
@@ -27144,7 +27129,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A177" s="9" t="s">
         <v>1574</v>
       </c>
@@ -27171,7 +27156,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A178" s="9" t="s">
         <v>1575</v>
       </c>
@@ -27198,7 +27183,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A179" s="9" t="s">
         <v>1576</v>
       </c>
@@ -27225,7 +27210,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A180" s="9" t="s">
         <v>1577</v>
       </c>
@@ -27252,7 +27237,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A181" s="9" t="s">
         <v>1578</v>
       </c>
@@ -27279,7 +27264,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A182" s="9" t="s">
         <v>1579</v>
       </c>
@@ -27306,7 +27291,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A183" s="9" t="s">
         <v>1580</v>
       </c>
@@ -27333,7 +27318,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A184" s="9" t="s">
         <v>1581</v>
       </c>
@@ -27360,7 +27345,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A185" s="9" t="s">
         <v>1582</v>
       </c>
@@ -27387,7 +27372,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A186" s="9" t="s">
         <v>1583</v>
       </c>
@@ -27414,7 +27399,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A187" s="9" t="s">
         <v>1584</v>
       </c>
@@ -27441,7 +27426,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A188" s="9" t="s">
         <v>1585</v>
       </c>
@@ -27468,7 +27453,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A189" s="9" t="s">
         <v>1586</v>
       </c>
@@ -27495,7 +27480,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A190" s="9" t="s">
         <v>1587</v>
       </c>
@@ -27522,7 +27507,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A191" s="9" t="s">
         <v>1588</v>
       </c>
@@ -27579,10 +27564,13 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
@@ -27595,10 +27583,10 @@
         <v>807</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>1791</v>
+        <v>1784</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -27612,7 +27600,7 @@
         <v>319</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>1905</v>
+        <v>1862</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>319</v>
@@ -27649,10 +27637,10 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20" t="s">
-        <v>1710</v>
+        <v>1882</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -27664,7 +27652,7 @@
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20" t="s">
-        <v>1755</v>
+        <v>1883</v>
       </c>
       <c r="E6" s="20"/>
     </row>
@@ -27676,7 +27664,6 @@
         <v>1679</v>
       </c>
       <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -27818,14 +27805,14 @@
         <v>1709</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>1827</v>
+        <v>1807</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20" t="s">
-        <v>1828</v>
+        <v>1884</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>1829</v>
+        <v>1808</v>
       </c>
     </row>
   </sheetData>
@@ -27838,17 +27825,20 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1889</v>
+        <v>1846</v>
       </c>
       <c r="B1" t="s">
-        <v>1791</v>
+        <v>1784</v>
       </c>
       <c r="C1" t="s">
         <v>807</v>
@@ -27856,10 +27846,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1888</v>
+        <v>1845</v>
       </c>
       <c r="B2" t="s">
-        <v>1905</v>
+        <v>1862</v>
       </c>
       <c r="C2" t="s">
         <v>319</v>
@@ -27867,167 +27857,167 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1890</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1858</v>
+        <v>1847</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1885</v>
       </c>
       <c r="C3" t="s">
-        <v>1859</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1891</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1860</v>
+        <v>1848</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>1886</v>
       </c>
       <c r="C4" t="s">
-        <v>1861</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1892</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1862</v>
+        <v>1849</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>1887</v>
       </c>
       <c r="C5" t="s">
-        <v>1863</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1893</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1864</v>
+        <v>1850</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>1888</v>
       </c>
       <c r="C6" t="s">
-        <v>1865</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1894</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1866</v>
+        <v>1851</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>1889</v>
       </c>
       <c r="C7" t="s">
-        <v>1867</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1895</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1868</v>
+        <v>1852</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>1890</v>
       </c>
       <c r="C8" t="s">
-        <v>1869</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1896</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1870</v>
+        <v>1853</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>1891</v>
       </c>
       <c r="C9" t="s">
-        <v>1871</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1897</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1872</v>
+        <v>1854</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>1892</v>
       </c>
       <c r="C10" t="s">
-        <v>1873</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1898</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1874</v>
+        <v>1855</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>1893</v>
       </c>
       <c r="C11" t="s">
-        <v>1875</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1899</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1876</v>
+        <v>1856</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>1894</v>
       </c>
       <c r="C12" t="s">
-        <v>1877</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1900</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1878</v>
+        <v>1857</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>1895</v>
       </c>
       <c r="C13" t="s">
-        <v>1879</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1901</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1880</v>
+        <v>1858</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>1896</v>
       </c>
       <c r="C14" t="s">
-        <v>1881</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1902</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1882</v>
+        <v>1859</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>1897</v>
       </c>
       <c r="C15" t="s">
-        <v>1883</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1903</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1884</v>
+        <v>1860</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>1898</v>
       </c>
       <c r="C16" t="s">
-        <v>1885</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1904</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1886</v>
+        <v>1861</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>1899</v>
       </c>
       <c r="C17" t="s">
-        <v>1887</v>
+        <v>1844</v>
       </c>
     </row>
   </sheetData>
@@ -28037,87 +28027,64 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B1" t="s">
         <v>1589</v>
       </c>
       <c r="C1" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D1" t="s">
         <v>1729</v>
       </c>
-      <c r="D1" t="s">
-        <v>1731</v>
-      </c>
       <c r="E1" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="F1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="G1" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
       <c r="H1" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B2" t="s">
         <v>319</v>
       </c>
       <c r="C2" t="s">
-        <v>1730</v>
+        <v>1862</v>
       </c>
       <c r="D2" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="E2" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="F2" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="G2" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="H2" t="s">
         <v>706</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>1754</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1754</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1753</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1753</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1752</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1718</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed errors in data for use in Arch.adl
</commit_message>
<xml_diff>
--- a/Blik/ProductCodes.xlsx
+++ b/Blik/ProductCodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="12195" windowHeight="6510" tabRatio="731" firstSheet="4" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="270" windowWidth="12195" windowHeight="6450" tabRatio="731" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Strategische planning" sheetId="1" r:id="rId1"/>
@@ -19322,7 +19322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19478,8 +19478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add dienstverbanden to Arch.adl
</commit_message>
<xml_diff>
--- a/Blik/ProductCodes.xlsx
+++ b/Blik/ProductCodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="270" windowWidth="12195" windowHeight="6450" tabRatio="731" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="12195" windowHeight="6390" tabRatio="731" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Strategische planning" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4751" uniqueCount="1908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4787" uniqueCount="1922">
   <si>
     <t>Divisie</t>
   </si>
@@ -5466,39 +5466,12 @@
     <t>Een vergunning is een beschikking waarin aan een persoon een afwijking op regelgeving wordt toegestaan of een bij regelgeving vereiste toestemming wordt verleend.</t>
   </si>
   <si>
-    <t>o1</t>
-  </si>
-  <si>
-    <t>o2</t>
-  </si>
-  <si>
-    <t>o3</t>
-  </si>
-  <si>
-    <t>o4</t>
-  </si>
-  <si>
-    <t>o5</t>
-  </si>
-  <si>
-    <t>o6</t>
-  </si>
-  <si>
-    <t>o7</t>
-  </si>
-  <si>
-    <t>o8</t>
-  </si>
-  <si>
     <t>Nederlandse Voedsel- en Warenautoriteit</t>
   </si>
   <si>
     <t>Bureau Risicobeoordeling en Onderzoeksprogrammering</t>
   </si>
   <si>
-    <t>Divisie Klatcontact en Dienstverlening</t>
-  </si>
-  <si>
     <t>Divisie Veterinair en Import</t>
   </si>
   <si>
@@ -5761,6 +5734,75 @@
   </si>
   <si>
     <t>524</t>
+  </si>
+  <si>
+    <t>taak</t>
+  </si>
+  <si>
+    <t>[Taak,]</t>
+  </si>
+  <si>
+    <t>taak12,taak13</t>
+  </si>
+  <si>
+    <t>taak2,taak3</t>
+  </si>
+  <si>
+    <t>taak2,taak7,taak11</t>
+  </si>
+  <si>
+    <t>taak7,taak8,taak9</t>
+  </si>
+  <si>
+    <t>NVWA IG en Plv IG</t>
+  </si>
+  <si>
+    <t>NVWA 05 VWNW kandidaten</t>
+  </si>
+  <si>
+    <t>Divisie Klantcontact en Dienstverlening</t>
+  </si>
+  <si>
+    <t>Directie Bedrijfsvoering</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>IG</t>
+  </si>
+  <si>
+    <t>63070166</t>
+  </si>
+  <si>
+    <t>63070170</t>
+  </si>
+  <si>
+    <t>63070171</t>
+  </si>
+  <si>
+    <t>63070172</t>
+  </si>
+  <si>
+    <t>63070173</t>
+  </si>
+  <si>
+    <t>63070174</t>
+  </si>
+  <si>
+    <t>63070175</t>
+  </si>
+  <si>
+    <t>63070169</t>
+  </si>
+  <si>
+    <t>63070168</t>
+  </si>
+  <si>
+    <t>63287511</t>
+  </si>
+  <si>
+    <t>63287555</t>
   </si>
 </sst>
 </file>
@@ -5878,7 +5920,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -5920,6 +5962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -19158,7 +19201,7 @@
         <v>985</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>1862</v>
+        <v>1853</v>
       </c>
       <c r="C2" t="s">
         <v>319</v>
@@ -19169,7 +19212,7 @@
         <v>1786</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1869</v>
+        <v>1860</v>
       </c>
       <c r="C3" t="s">
         <v>1777</v>
@@ -19180,7 +19223,7 @@
         <v>1787</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1870</v>
+        <v>1861</v>
       </c>
       <c r="C4" t="s">
         <v>1778</v>
@@ -19191,7 +19234,7 @@
         <v>1788</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>1871</v>
+        <v>1862</v>
       </c>
       <c r="C5" t="s">
         <v>1799</v>
@@ -19202,7 +19245,7 @@
         <v>1789</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>1872</v>
+        <v>1863</v>
       </c>
       <c r="C6" t="s">
         <v>1800</v>
@@ -19213,7 +19256,7 @@
         <v>1790</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>1873</v>
+        <v>1864</v>
       </c>
       <c r="C7" t="s">
         <v>1801</v>
@@ -19224,7 +19267,7 @@
         <v>1791</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>1874</v>
+        <v>1865</v>
       </c>
       <c r="C8" t="s">
         <v>1779</v>
@@ -19235,7 +19278,7 @@
         <v>1792</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>1875</v>
+        <v>1866</v>
       </c>
       <c r="C9" t="s">
         <v>1780</v>
@@ -19246,7 +19289,7 @@
         <v>1793</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>1876</v>
+        <v>1867</v>
       </c>
       <c r="C10" t="s">
         <v>1802</v>
@@ -19260,7 +19303,7 @@
         <v>1794</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>1877</v>
+        <v>1868</v>
       </c>
       <c r="C11" t="s">
         <v>1782</v>
@@ -19274,7 +19317,7 @@
         <v>1795</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>1878</v>
+        <v>1869</v>
       </c>
       <c r="C12" t="s">
         <v>1803</v>
@@ -19285,7 +19328,7 @@
         <v>1796</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>1879</v>
+        <v>1870</v>
       </c>
       <c r="C13" t="s">
         <v>1804</v>
@@ -19296,7 +19339,7 @@
         <v>1797</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>1880</v>
+        <v>1871</v>
       </c>
       <c r="C14" t="s">
         <v>1805</v>
@@ -19307,7 +19350,7 @@
         <v>1798</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>1881</v>
+        <v>1872</v>
       </c>
       <c r="C15" t="s">
         <v>1806</v>
@@ -19320,154 +19363,233 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1865</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>807</v>
       </c>
-      <c r="C1" t="s">
-        <v>1828</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="20" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1864</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="D2" t="s">
-        <v>1862</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2" s="20" t="s">
+        <v>1853</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>1809</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>1891</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>1892</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>1893</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>1812</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>1894</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>1895</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>1896</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>1817</v>
       </c>
-      <c r="C3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1810</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1818</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1827</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1819</v>
-      </c>
-      <c r="C5" t="s">
-        <v>816</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1902</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1812</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C9" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>1820</v>
       </c>
-      <c r="C6" t="s">
-        <v>1821</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1903</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>1813</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1822</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1823</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1814</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1824</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1825</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C10" s="20" t="s">
+        <v>1857</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>1898</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>1905</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1815</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1826</v>
-      </c>
-      <c r="C9" t="s">
-        <v>298</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C11" s="20" t="s">
+        <v>1910</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>1908</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>1906</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1816</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1829</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1866</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1907</v>
-      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19478,7 +19600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A27"/>
     </sheetView>
   </sheetViews>
@@ -19838,10 +19960,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B247"/>
+  <dimension ref="A1:C247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B247"/>
+    <sheetView topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231:C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19868,439 +19990,439 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>813</v>
+        <v>860</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>814</v>
+        <v>956</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>816</v>
+        <v>875</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>817</v>
+        <v>888</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>818</v>
+        <v>920</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>819</v>
+        <v>826</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>820</v>
+        <v>858</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>271</v>
       </c>
       <c r="B11" t="s">
-        <v>821</v>
+        <v>848</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>822</v>
+        <v>936</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>823</v>
+        <v>935</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>824</v>
+        <v>907</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>815</v>
+        <v>906</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>825</v>
+        <v>952</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="B17" t="s">
-        <v>816</v>
+        <v>840</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="B18" t="s">
-        <v>826</v>
+        <v>919</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>827</v>
+        <v>931</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>828</v>
+        <v>961</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
-        <v>829</v>
+        <v>844</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B22" t="s">
-        <v>830</v>
+        <v>844</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
-        <v>824</v>
+        <v>878</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>831</v>
+        <v>924</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>815</v>
+        <v>855</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>833</v>
+        <v>863</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>711</v>
+        <v>911</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>207</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>834</v>
+        <v>853</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>835</v>
+        <v>853</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>212</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>836</v>
+        <v>853</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>204</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>837</v>
+        <v>862</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="B33" t="s">
-        <v>838</v>
+        <v>883</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
-        <v>839</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="B35" t="s">
-        <v>840</v>
+        <v>904</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="B36" t="s">
-        <v>834</v>
+        <v>910</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>224</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
-        <v>841</v>
+        <v>963</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>221</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
-        <v>842</v>
+        <v>966</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>967</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>965</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>843</v>
+        <v>964</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>844</v>
+        <v>968</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>225</v>
+        <v>141</v>
       </c>
       <c r="B44" t="s">
-        <v>845</v>
+        <v>969</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>827</v>
+        <v>849</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>223</v>
+        <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>847</v>
+        <v>859</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>271</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>848</v>
+        <v>857</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>849</v>
+        <v>838</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
-        <v>850</v>
+        <v>929</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="B51" t="s">
-        <v>851</v>
+        <v>927</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>834</v>
+        <v>928</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>842</v>
+        <v>877</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>852</v>
+        <v>819</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
-        <v>853</v>
+        <v>932</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>174</v>
       </c>
       <c r="B56" t="s">
-        <v>854</v>
+        <v>934</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
         <v>823</v>
@@ -20308,74 +20430,74 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>855</v>
+        <v>823</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
-        <v>856</v>
+        <v>839</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>244</v>
       </c>
       <c r="B60" t="s">
-        <v>831</v>
+        <v>882</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>246</v>
       </c>
       <c r="B61" t="s">
-        <v>857</v>
+        <v>885</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>247</v>
       </c>
       <c r="B62" t="s">
-        <v>858</v>
+        <v>881</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>248</v>
       </c>
       <c r="B63" t="s">
-        <v>859</v>
+        <v>889</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>156</v>
+        <v>249</v>
       </c>
       <c r="B64" t="s">
-        <v>816</v>
+        <v>884</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>815</v>
+        <v>890</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>250</v>
       </c>
       <c r="B66" t="s">
-        <v>860</v>
+        <v>887</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -20396,207 +20518,207 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>251</v>
       </c>
       <c r="B69" t="s">
-        <v>862</v>
+        <v>891</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>158</v>
+        <v>272</v>
       </c>
       <c r="B70" t="s">
-        <v>827</v>
+        <v>891</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>863</v>
+        <v>914</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>273</v>
       </c>
       <c r="B72" t="s">
-        <v>864</v>
+        <v>914</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="B73" t="s">
-        <v>816</v>
+        <v>903</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>865</v>
+        <v>955</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
-        <v>866</v>
+        <v>816</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="B77" t="s">
-        <v>842</v>
+        <v>816</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>288</v>
+        <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>267</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="B80" t="s">
-        <v>842</v>
+        <v>816</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>234</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>867</v>
+        <v>816</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>233</v>
+        <v>165</v>
       </c>
       <c r="B82" t="s">
-        <v>868</v>
+        <v>816</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>237</v>
+        <v>142</v>
       </c>
       <c r="B83" t="s">
-        <v>869</v>
+        <v>816</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="B84" t="s">
-        <v>870</v>
+        <v>842</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>236</v>
+        <v>52</v>
       </c>
       <c r="B85" t="s">
-        <v>871</v>
+        <v>842</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>235</v>
+        <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>815</v>
+        <v>842</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B87" t="s">
-        <v>820</v>
+        <v>842</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>34</v>
       </c>
       <c r="B88" t="s">
-        <v>834</v>
+        <v>842</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>33</v>
+        <v>252</v>
       </c>
       <c r="B89" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B90" t="s">
-        <v>872</v>
+        <v>842</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>873</v>
+        <v>842</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>39</v>
+        <v>274</v>
       </c>
       <c r="B92" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B93" t="s">
-        <v>834</v>
+        <v>842</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="B94" t="s">
         <v>842</v>
@@ -20604,87 +20726,87 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>31</v>
+        <v>207</v>
       </c>
       <c r="B95" t="s">
-        <v>853</v>
+        <v>834</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>37</v>
+        <v>222</v>
       </c>
       <c r="B96" t="s">
-        <v>874</v>
+        <v>834</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>875</v>
+        <v>834</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>122</v>
+        <v>231</v>
       </c>
       <c r="B98" t="s">
-        <v>876</v>
+        <v>834</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="B99" t="s">
-        <v>877</v>
+        <v>834</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B100" t="s">
-        <v>878</v>
+        <v>834</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>253</v>
       </c>
       <c r="B101" t="s">
-        <v>824</v>
+        <v>834</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="B102" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="B103" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>815</v>
+        <v>834</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B105" t="s">
         <v>834</v>
@@ -20692,31 +20814,31 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>275</v>
       </c>
       <c r="B106" t="s">
-        <v>879</v>
+        <v>834</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="B107" t="s">
-        <v>815</v>
+        <v>834</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>253</v>
+        <v>166</v>
       </c>
       <c r="B108" t="s">
-        <v>834</v>
+        <v>926</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>254</v>
+        <v>26</v>
       </c>
       <c r="B109" t="s">
         <v>820</v>
@@ -20724,439 +20846,439 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B110" t="s">
-        <v>842</v>
+        <v>820</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B111" t="s">
-        <v>880</v>
+        <v>820</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>247</v>
+        <v>71</v>
       </c>
       <c r="B112" t="s">
-        <v>881</v>
+        <v>820</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>244</v>
+        <v>98</v>
       </c>
       <c r="B113" t="s">
-        <v>882</v>
+        <v>820</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>243</v>
+        <v>80</v>
       </c>
       <c r="B114" t="s">
-        <v>883</v>
+        <v>899</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>249</v>
+        <v>54</v>
       </c>
       <c r="B115" t="s">
-        <v>884</v>
+        <v>850</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>246</v>
+        <v>36</v>
       </c>
       <c r="B116" t="s">
-        <v>885</v>
+        <v>873</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>265</v>
+        <v>27</v>
       </c>
       <c r="B117" t="s">
-        <v>886</v>
+        <v>821</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>250</v>
+        <v>72</v>
       </c>
       <c r="B118" t="s">
-        <v>887</v>
+        <v>821</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>240</v>
+        <v>99</v>
       </c>
       <c r="B119" t="s">
-        <v>888</v>
+        <v>821</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>248</v>
+        <v>63</v>
       </c>
       <c r="B120" t="s">
-        <v>889</v>
+        <v>864</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="B121" t="s">
-        <v>890</v>
+        <v>817</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>251</v>
+        <v>86</v>
       </c>
       <c r="B122" t="s">
-        <v>891</v>
+        <v>916</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="B123" t="s">
-        <v>892</v>
+        <v>947</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>259</v>
+        <v>100</v>
       </c>
       <c r="B124" t="s">
-        <v>893</v>
+        <v>951</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>264</v>
+        <v>223</v>
       </c>
       <c r="B125" t="s">
-        <v>894</v>
+        <v>846</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="B126" t="s">
-        <v>895</v>
+        <v>868</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="B127" t="s">
-        <v>896</v>
+        <v>867</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="B128" t="s">
-        <v>897</v>
+        <v>828</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B129" t="s">
-        <v>815</v>
+        <v>876</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B130" t="s">
-        <v>816</v>
+        <v>898</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>898</v>
+        <v>822</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>80</v>
+        <v>277</v>
       </c>
       <c r="B132" t="s">
-        <v>899</v>
+        <v>944</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>82</v>
+        <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>900</v>
+        <v>940</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="B134" t="s">
-        <v>901</v>
+        <v>939</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="B135" t="s">
-        <v>902</v>
+        <v>957</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="B136" t="s">
-        <v>903</v>
+        <v>874</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="B137" t="s">
-        <v>904</v>
+        <v>925</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>55</v>
       </c>
       <c r="B138" t="s">
-        <v>905</v>
+        <v>852</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="B139" t="s">
-        <v>816</v>
+        <v>830</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>194</v>
       </c>
       <c r="B140" t="s">
-        <v>815</v>
+        <v>843</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B141" t="s">
-        <v>906</v>
+        <v>854</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>181</v>
+        <v>38</v>
       </c>
       <c r="B142" t="s">
-        <v>907</v>
+        <v>872</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>187</v>
+        <v>87</v>
       </c>
       <c r="B143" t="s">
-        <v>908</v>
+        <v>917</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>255</v>
       </c>
       <c r="B144" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>258</v>
+        <v>113</v>
       </c>
       <c r="B145" t="s">
-        <v>871</v>
+        <v>825</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>184</v>
+        <v>256</v>
       </c>
       <c r="B146" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B147" t="s">
-        <v>827</v>
+        <v>908</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="B148" t="s">
-        <v>856</v>
+        <v>866</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
       <c r="B149" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B150" t="s">
-        <v>853</v>
+        <v>900</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B151" t="s">
-        <v>821</v>
+        <v>958</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>70</v>
+        <v>280</v>
       </c>
       <c r="B152" t="s">
-        <v>834</v>
+        <v>943</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>71</v>
+        <v>281</v>
       </c>
       <c r="B153" t="s">
-        <v>820</v>
+        <v>945</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>842</v>
+        <v>815</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="B155" t="s">
-        <v>851</v>
+        <v>815</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>74</v>
+        <v>210</v>
       </c>
       <c r="B156" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>75</v>
+        <v>224</v>
       </c>
       <c r="B157" t="s">
-        <v>912</v>
+        <v>815</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>913</v>
+        <v>815</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>914</v>
+        <v>815</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="B160" t="s">
-        <v>915</v>
+        <v>815</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B161" t="s">
-        <v>916</v>
+        <v>815</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>87</v>
+        <v>257</v>
       </c>
       <c r="B162" t="s">
-        <v>917</v>
+        <v>815</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>918</v>
+        <v>815</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="B164" t="s">
         <v>815</v>
@@ -21164,58 +21286,58 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>815</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="B166" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="B167" t="s">
-        <v>919</v>
+        <v>815</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>241</v>
+        <v>144</v>
       </c>
       <c r="B168" t="s">
-        <v>920</v>
+        <v>815</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>268</v>
+        <v>57</v>
       </c>
       <c r="B169" t="s">
-        <v>921</v>
+        <v>851</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>256</v>
+        <v>39</v>
       </c>
       <c r="B170" t="s">
-        <v>922</v>
+        <v>851</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B171" t="s">
-        <v>923</v>
+        <v>851</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
@@ -21228,607 +21350,622 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="B173" t="s">
-        <v>924</v>
+        <v>851</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B174" t="s">
-        <v>834</v>
+        <v>818</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B175" t="s">
-        <v>925</v>
+        <v>818</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
       <c r="B176" t="s">
-        <v>856</v>
+        <v>950</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="B177" t="s">
-        <v>926</v>
+        <v>814</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="B178" t="s">
-        <v>927</v>
+        <v>933</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="B179" t="s">
-        <v>816</v>
+        <v>845</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>168</v>
+        <v>236</v>
       </c>
       <c r="B180" t="s">
-        <v>909</v>
+        <v>871</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
       <c r="B181" t="s">
-        <v>928</v>
+        <v>871</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B182" t="s">
-        <v>929</v>
+        <v>871</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>167</v>
+        <v>284</v>
       </c>
       <c r="B183" t="s">
-        <v>827</v>
+        <v>871</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="B184" t="s">
-        <v>930</v>
+        <v>827</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="B185" t="s">
-        <v>856</v>
+        <v>827</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B186" t="s">
-        <v>931</v>
+        <v>827</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="B187" t="s">
-        <v>932</v>
+        <v>827</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B188" t="s">
-        <v>834</v>
+        <v>827</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B189" t="s">
-        <v>842</v>
+        <v>827</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="B190" t="s">
-        <v>815</v>
+        <v>827</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="B191" t="s">
-        <v>933</v>
+        <v>711</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="B192" t="s">
-        <v>934</v>
+        <v>836</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>129</v>
+        <v>11</v>
       </c>
       <c r="B193" t="s">
-        <v>935</v>
+        <v>909</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="B194" t="s">
-        <v>834</v>
+        <v>909</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>131</v>
+        <v>259</v>
       </c>
       <c r="B195" t="s">
-        <v>936</v>
+        <v>893</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="B196" t="s">
-        <v>937</v>
+        <v>880</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B197" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>279</v>
+        <v>169</v>
       </c>
       <c r="B198" t="s">
-        <v>939</v>
+        <v>930</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B199" t="s">
-        <v>940</v>
+        <v>948</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>275</v>
+        <v>125</v>
       </c>
       <c r="B200" t="s">
-        <v>834</v>
+        <v>879</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>202</v>
+        <v>261</v>
       </c>
       <c r="B201" t="s">
-        <v>941</v>
+        <v>896</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>274</v>
+        <v>105</v>
       </c>
       <c r="B202" t="s">
-        <v>842</v>
+        <v>960</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="B203" t="s">
-        <v>942</v>
+        <v>829</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>280</v>
+        <v>90</v>
       </c>
       <c r="B204" t="s">
-        <v>943</v>
+        <v>918</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B205" t="s">
-        <v>815</v>
+        <v>962</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
       <c r="B206" t="s">
-        <v>944</v>
+        <v>847</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>272</v>
+        <v>214</v>
       </c>
       <c r="B207" t="s">
-        <v>891</v>
+        <v>833</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B208" t="s">
-        <v>945</v>
+        <v>897</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>273</v>
+        <v>202</v>
       </c>
       <c r="B209" t="s">
-        <v>914</v>
+        <v>941</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="B210" t="s">
-        <v>946</v>
+        <v>869</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B211" t="s">
-        <v>947</v>
+        <v>894</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="B212" t="s">
-        <v>948</v>
+        <v>886</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="B213" t="s">
-        <v>949</v>
+        <v>892</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>283</v>
+        <v>228</v>
       </c>
       <c r="B214" t="s">
-        <v>950</v>
+        <v>841</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>100</v>
+        <v>215</v>
       </c>
       <c r="B215" t="s">
-        <v>951</v>
+        <v>832</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>94</v>
+        <v>216</v>
       </c>
       <c r="B216" t="s">
-        <v>952</v>
+        <v>835</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="B217" t="s">
-        <v>953</v>
+        <v>870</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>96</v>
+        <v>287</v>
       </c>
       <c r="B218" t="s">
-        <v>842</v>
+        <v>946</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="B219" t="s">
-        <v>954</v>
+        <v>902</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="B220" t="s">
-        <v>955</v>
+        <v>856</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>99</v>
+        <v>189</v>
       </c>
       <c r="B221" t="s">
-        <v>821</v>
+        <v>856</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>97</v>
+        <v>170</v>
       </c>
       <c r="B222" t="s">
-        <v>834</v>
+        <v>856</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="B223" t="s">
-        <v>820</v>
+        <v>856</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B224" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
       <c r="B225" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>102</v>
+        <v>288</v>
       </c>
       <c r="B226" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>103</v>
+        <v>267</v>
       </c>
       <c r="B227" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
+        <v>126</v>
+      </c>
+      <c r="B228" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>289</v>
+      </c>
+      <c r="B229" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>75</v>
+      </c>
+      <c r="B230" t="s">
+        <v>912</v>
+      </c>
+      <c r="C230" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>76</v>
+      </c>
+      <c r="B231" t="s">
+        <v>915</v>
+      </c>
+      <c r="C231" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
         <v>106</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B232" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" t="s">
-        <v>105</v>
-      </c>
-      <c r="B229" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" t="s">
+      <c r="C232" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>107</v>
+      </c>
+      <c r="B233" t="s">
+        <v>954</v>
+      </c>
+      <c r="C233" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>77</v>
+      </c>
+      <c r="B234" t="s">
+        <v>913</v>
+      </c>
+      <c r="C234" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>290</v>
+      </c>
+      <c r="B235" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>195</v>
+      </c>
+      <c r="B236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>91</v>
+      </c>
+      <c r="B237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
         <v>201</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B238" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" t="s">
-        <v>198</v>
-      </c>
-      <c r="B231" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" t="s">
-        <v>200</v>
-      </c>
-      <c r="B232" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" t="s">
-        <v>262</v>
-      </c>
-      <c r="B233" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" t="s">
-        <v>133</v>
-      </c>
-      <c r="B234" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" t="s">
-        <v>137</v>
-      </c>
-      <c r="B235" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" t="s">
-        <v>144</v>
-      </c>
-      <c r="B236" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A237" t="s">
-        <v>136</v>
-      </c>
-      <c r="B237" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A238" t="s">
-        <v>134</v>
-      </c>
-      <c r="B238" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="B239" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="B240" t="s">
-        <v>816</v>
+        <v>831</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B241" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>135</v>
+        <v>268</v>
       </c>
       <c r="B242" t="s">
-        <v>967</v>
+        <v>921</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B243" t="s">
-        <v>968</v>
+        <v>831</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>145</v>
+        <v>291</v>
       </c>
       <c r="B244" t="s">
-        <v>871</v>
+        <v>949</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>284</v>
+        <v>46</v>
       </c>
       <c r="B245" t="s">
-        <v>871</v>
+        <v>923</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="B246" t="s">
-        <v>969</v>
+        <v>953</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>147</v>
+        <v>269</v>
       </c>
       <c r="B247" t="s">
-        <v>831</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B381">
-    <sortCondition ref="A3:A381"/>
+  <sortState ref="A3:B247">
+    <sortCondition ref="B3:B247"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21836,18 +21973,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>808</v>
       </c>
@@ -21866,8 +22004,11 @@
       <c r="F1" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>809</v>
       </c>
@@ -21886,8 +22027,11 @@
       <c r="F2" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>717</v>
       </c>
@@ -21903,8 +22047,11 @@
       <c r="F3" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>743</v>
       </c>
@@ -21915,7 +22062,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>744</v>
       </c>
@@ -21926,7 +22073,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>762</v>
       </c>
@@ -21937,7 +22084,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>763</v>
       </c>
@@ -21948,7 +22095,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>764</v>
       </c>
@@ -21959,7 +22106,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>745</v>
       </c>
@@ -21970,7 +22117,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>729</v>
       </c>
@@ -21989,8 +22136,11 @@
       <c r="F10" t="s">
         <v>976</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>731</v>
       </c>
@@ -22009,8 +22159,11 @@
       <c r="F11" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>740</v>
       </c>
@@ -22030,7 +22183,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>741</v>
       </c>
@@ -22050,7 +22203,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>719</v>
       </c>
@@ -22069,8 +22222,11 @@
       <c r="F14" t="s">
         <v>974</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>768</v>
       </c>
@@ -22081,8 +22237,11 @@
         <v>751</v>
       </c>
       <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>769</v>
       </c>
@@ -22093,8 +22252,11 @@
         <v>751</v>
       </c>
       <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>770</v>
       </c>
@@ -22105,8 +22267,11 @@
         <v>751</v>
       </c>
       <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>771</v>
       </c>
@@ -22117,8 +22282,11 @@
         <v>751</v>
       </c>
       <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>721</v>
       </c>
@@ -22138,7 +22306,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>727</v>
       </c>
@@ -22157,8 +22325,11 @@
       <c r="F20" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>776</v>
       </c>
@@ -22169,8 +22340,11 @@
         <v>751</v>
       </c>
       <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>777</v>
       </c>
@@ -22181,8 +22355,11 @@
         <v>751</v>
       </c>
       <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>723</v>
       </c>
@@ -22201,8 +22378,11 @@
       <c r="F23" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>780</v>
       </c>
@@ -22213,8 +22393,11 @@
         <v>751</v>
       </c>
       <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>781</v>
       </c>
@@ -22225,8 +22408,11 @@
         <v>751</v>
       </c>
       <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>782</v>
       </c>
@@ -22237,8 +22423,11 @@
         <v>751</v>
       </c>
       <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>725</v>
       </c>
@@ -22257,8 +22446,11 @@
       <c r="F27" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>786</v>
       </c>
@@ -22269,8 +22461,11 @@
         <v>751</v>
       </c>
       <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>787</v>
       </c>
@@ -22281,8 +22476,11 @@
         <v>751</v>
       </c>
       <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>788</v>
       </c>
@@ -22293,8 +22491,11 @@
         <v>751</v>
       </c>
       <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>733</v>
       </c>
@@ -22308,7 +22509,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>792</v>
       </c>
@@ -22319,7 +22520,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>793</v>
       </c>
@@ -22330,7 +22531,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>794</v>
       </c>
@@ -22341,7 +22542,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>728</v>
       </c>
@@ -22352,7 +22553,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>798</v>
       </c>
@@ -22363,7 +22564,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>799</v>
       </c>
@@ -22374,7 +22575,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>800</v>
       </c>
@@ -22385,7 +22586,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>735</v>
       </c>
@@ -22405,7 +22606,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>738</v>
       </c>
@@ -22425,7 +22626,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>737</v>
       </c>
@@ -22442,7 +22643,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>739</v>
       </c>
@@ -22462,7 +22663,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>753</v>
       </c>
@@ -22472,8 +22673,11 @@
       <c r="C43" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>754</v>
       </c>
@@ -22483,8 +22687,11 @@
       <c r="C44" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D45">
         <f>SUM(D3:D44)</f>
         <v>2625227</v>
@@ -22612,7 +22819,7 @@
         <v>987</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>1238</v>
@@ -22639,7 +22846,7 @@
         <v>987</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>1239</v>
@@ -23102,7 +23309,7 @@
         <v>987</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>1241</v>
@@ -23129,7 +23336,7 @@
         <v>987</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>1241</v>
@@ -23811,7 +24018,7 @@
         <v>1022</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>1245</v>
@@ -23917,7 +24124,7 @@
         <v>1022</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>1248</v>
@@ -24083,7 +24290,7 @@
         <v>1022</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>1250</v>
@@ -24108,7 +24315,7 @@
         <v>1044</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>1867</v>
+        <v>1858</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>1223</v>
@@ -24135,7 +24342,7 @@
         <v>1044</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>1867</v>
+        <v>1858</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>1226</v>
@@ -24162,7 +24369,7 @@
         <v>1044</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>1252</v>
@@ -24243,7 +24450,7 @@
         <v>1044</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>1867</v>
+        <v>1858</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>1229</v>
@@ -24293,7 +24500,7 @@
         <v>1044</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>1867</v>
+        <v>1858</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>1231</v>
@@ -24320,7 +24527,7 @@
         <v>1044</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>1256</v>
@@ -24457,7 +24664,7 @@
         <v>1044</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>1258</v>
@@ -24484,7 +24691,7 @@
         <v>1044</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>1867</v>
+        <v>1858</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>1234</v>
@@ -24511,7 +24718,7 @@
         <v>1044</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>1260</v>
@@ -24540,7 +24747,7 @@
         <v>1044</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>1263</v>
@@ -24569,7 +24776,7 @@
         <v>1044</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>1867</v>
+        <v>1858</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>1236</v>
@@ -24596,7 +24803,7 @@
         <v>1044</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>1266</v>
@@ -24623,7 +24830,7 @@
         <v>1044</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>1268</v>
@@ -24650,7 +24857,7 @@
         <v>1044</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>1270</v>
@@ -24679,7 +24886,7 @@
         <v>1044</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>1273</v>
@@ -24733,7 +24940,7 @@
         <v>1044</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>1276</v>
@@ -24758,7 +24965,7 @@
         <v>1044</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>1868</v>
+        <v>1859</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>1280</v>
@@ -24785,7 +24992,7 @@
         <v>1044</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>1863</v>
+        <v>1854</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>1277</v>
@@ -27600,7 +27807,7 @@
         <v>319</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>1862</v>
+        <v>1853</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>319</v>
@@ -27637,7 +27844,7 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20" t="s">
-        <v>1882</v>
+        <v>1873</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>1711</v>
@@ -27652,7 +27859,7 @@
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20" t="s">
-        <v>1883</v>
+        <v>1874</v>
       </c>
       <c r="E6" s="20"/>
     </row>
@@ -27809,7 +28016,7 @@
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20" t="s">
-        <v>1884</v>
+        <v>1875</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>1808</v>
@@ -27825,7 +28032,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27835,7 +28042,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1846</v>
+        <v>1837</v>
       </c>
       <c r="B1" t="s">
         <v>1784</v>
@@ -27846,10 +28053,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1845</v>
+        <v>1836</v>
       </c>
       <c r="B2" t="s">
-        <v>1862</v>
+        <v>1853</v>
       </c>
       <c r="C2" t="s">
         <v>319</v>
@@ -27857,167 +28064,167 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1847</v>
+        <v>1838</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1885</v>
+        <v>1876</v>
       </c>
       <c r="C3" t="s">
-        <v>1830</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1848</v>
+        <v>1839</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1886</v>
+        <v>1877</v>
       </c>
       <c r="C4" t="s">
-        <v>1831</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1849</v>
+        <v>1840</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>1887</v>
+        <v>1878</v>
       </c>
       <c r="C5" t="s">
-        <v>1832</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1850</v>
+        <v>1841</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>1888</v>
+        <v>1879</v>
       </c>
       <c r="C6" t="s">
-        <v>1833</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1851</v>
+        <v>1842</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>1889</v>
+        <v>1880</v>
       </c>
       <c r="C7" t="s">
-        <v>1834</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1852</v>
+        <v>1843</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>1890</v>
+        <v>1881</v>
       </c>
       <c r="C8" t="s">
-        <v>1835</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1853</v>
+        <v>1844</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>1891</v>
+        <v>1882</v>
       </c>
       <c r="C9" t="s">
-        <v>1836</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1854</v>
+        <v>1845</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>1892</v>
+        <v>1883</v>
       </c>
       <c r="C10" t="s">
-        <v>1837</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1855</v>
+        <v>1846</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>1893</v>
+        <v>1884</v>
       </c>
       <c r="C11" t="s">
-        <v>1838</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1856</v>
+        <v>1847</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>1894</v>
+        <v>1885</v>
       </c>
       <c r="C12" t="s">
-        <v>1839</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1857</v>
+        <v>1848</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>1895</v>
+        <v>1886</v>
       </c>
       <c r="C13" t="s">
-        <v>1840</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1858</v>
+        <v>1849</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>1896</v>
+        <v>1887</v>
       </c>
       <c r="C14" t="s">
-        <v>1841</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1859</v>
+        <v>1850</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>1897</v>
+        <v>1888</v>
       </c>
       <c r="C15" t="s">
-        <v>1842</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1860</v>
+        <v>1851</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>1898</v>
+        <v>1889</v>
       </c>
       <c r="C16" t="s">
-        <v>1843</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1861</v>
+        <v>1852</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>1899</v>
+        <v>1890</v>
       </c>
       <c r="C17" t="s">
-        <v>1844</v>
+        <v>1835</v>
       </c>
     </row>
   </sheetData>
@@ -28069,7 +28276,7 @@
         <v>319</v>
       </c>
       <c r="C2" t="s">
-        <v>1862</v>
+        <v>1853</v>
       </c>
       <c r="D2" t="s">
         <v>1731</v>

</xml_diff>